<commit_message>
CIAA-ACC V1.1D. Changes in solder mask and solder paste layers (requested by manufacturer).
</commit_message>
<xml_diff>
--- a/PCB/ACC/CIAA_ACC/doc/stackup/stackup_top_bottom.xlsx
+++ b/PCB/ACC/CIAA_ACC/doc/stackup/stackup_top_bottom.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="53">
   <si>
     <t xml:space="preserve">L1</t>
   </si>
@@ -31,6 +31,9 @@
   </si>
   <si>
     <t xml:space="preserve">1oz +Plating</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primer stackup entregado por EDADOC, sólo se usaron de aquí los anchos de pista de los layers top y bottom.</t>
   </si>
   <si>
     <r>
@@ -51,6 +54,7 @@
         <color rgb="FF558ED5"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">（</t>
     </r>
@@ -72,6 +76,7 @@
         <color rgb="FF558ED5"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">）</t>
     </r>
@@ -101,6 +106,7 @@
         <color rgb="FF558ED5"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">（</t>
     </r>
@@ -122,6 +128,7 @@
         <color rgb="FF558ED5"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">）</t>
     </r>
@@ -148,6 +155,7 @@
         <color rgb="FF558ED5"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">（</t>
     </r>
@@ -169,6 +177,7 @@
         <color rgb="FF558ED5"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">）</t>
     </r>
@@ -201,6 +210,7 @@
         <color rgb="FF558ED5"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">（</t>
     </r>
@@ -222,6 +232,7 @@
         <color rgb="FF558ED5"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">）</t>
     </r>
@@ -352,7 +363,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -384,15 +395,9 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <b val="true"/>
+      <sz val="15"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
@@ -403,6 +408,7 @@
       <color rgb="FF558ED5"/>
       <name val="Droid Sans Fallback"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -433,24 +439,12 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor rgb="FFFCD5B5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor rgb="FFFFFF99"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -461,7 +455,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFCD5B5"/>
-        <bgColor rgb="FFFFC7CE"/>
+        <bgColor rgb="FFD9D9D9"/>
       </patternFill>
     </fill>
     <fill>
@@ -485,7 +479,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF99"/>
-        <bgColor rgb="FFFFEB9C"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -631,7 +625,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -655,30 +649,24 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="2" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="3" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -686,19 +674,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="5" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="2" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="6" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="7" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -706,43 +698,39 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="6" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="6" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="6" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="3" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="6" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="6" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="9" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="11" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -750,31 +738,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="7" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="7" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="5" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -782,15 +766,27 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="8" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="6" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="8" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="6" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="8" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="6" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="7" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -798,41 +794,27 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="7" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="9" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="9" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="7" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Bad" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Neutral" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Good" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -844,17 +826,17 @@
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF9C0006"/>
+      <rgbColor rgb="FF800000"/>
       <rgbColor rgb="FF006100"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF9C6500"/>
+      <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFEB9C"/>
+      <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFC6EFCE"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
@@ -873,7 +855,7 @@
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFFC7CE"/>
+      <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFCD5B5"/>
       <rgbColor rgb="FF3366FF"/>
@@ -903,14 +885,14 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>371520</xdr:colOff>
-      <xdr:row>93</xdr:row>
-      <xdr:rowOff>9360</xdr:rowOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>177840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>552240</xdr:colOff>
+      <xdr:colOff>551520</xdr:colOff>
       <xdr:row>107</xdr:row>
-      <xdr:rowOff>56520</xdr:rowOff>
+      <xdr:rowOff>41400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -923,8 +905,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7724520" y="18343080"/>
-          <a:ext cx="7534080" cy="2607480"/>
+          <a:off x="7709400" y="18343080"/>
+          <a:ext cx="7518240" cy="2606760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -941,13 +923,13 @@
       <xdr:col>12</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
       <xdr:row>62</xdr:row>
-      <xdr:rowOff>104760</xdr:rowOff>
+      <xdr:rowOff>90360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>605520</xdr:colOff>
+      <xdr:colOff>604800</xdr:colOff>
       <xdr:row>76</xdr:row>
-      <xdr:rowOff>142560</xdr:rowOff>
+      <xdr:rowOff>127440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -960,8 +942,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7810200" y="12769200"/>
-          <a:ext cx="7501680" cy="2598120"/>
+          <a:off x="7795080" y="12769200"/>
+          <a:ext cx="7485840" cy="2597400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -978,13 +960,13 @@
       <xdr:col>25</xdr:col>
       <xdr:colOff>89640</xdr:colOff>
       <xdr:row>62</xdr:row>
-      <xdr:rowOff>45000</xdr:rowOff>
+      <xdr:rowOff>30600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
-      <xdr:colOff>308520</xdr:colOff>
+      <xdr:colOff>307800</xdr:colOff>
       <xdr:row>76</xdr:row>
-      <xdr:rowOff>82800</xdr:rowOff>
+      <xdr:rowOff>67680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -997,8 +979,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15408720" y="12709440"/>
-          <a:ext cx="7572240" cy="2598120"/>
+          <a:off x="15377040" y="12709440"/>
+          <a:ext cx="7556400" cy="2597400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1015,13 +997,13 @@
       <xdr:col>37</xdr:col>
       <xdr:colOff>549000</xdr:colOff>
       <xdr:row>61</xdr:row>
-      <xdr:rowOff>156960</xdr:rowOff>
+      <xdr:rowOff>142560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>50</xdr:col>
-      <xdr:colOff>36360</xdr:colOff>
+      <xdr:colOff>35640</xdr:colOff>
       <xdr:row>76</xdr:row>
-      <xdr:rowOff>26640</xdr:rowOff>
+      <xdr:rowOff>11520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1034,8 +1016,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="23221440" y="12638520"/>
-          <a:ext cx="7453440" cy="2612880"/>
+          <a:off x="23174640" y="12638520"/>
+          <a:ext cx="7436160" cy="2612160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1052,13 +1034,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>134640</xdr:colOff>
       <xdr:row>92</xdr:row>
-      <xdr:rowOff>145800</xdr:rowOff>
+      <xdr:rowOff>131400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>296280</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>105</xdr:row>
-      <xdr:rowOff>129600</xdr:rowOff>
+      <xdr:rowOff>114480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1072,7 +1054,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="134640" y="18296640"/>
-          <a:ext cx="7514640" cy="2361240"/>
+          <a:ext cx="7498800" cy="2360520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1089,13 +1071,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>62</xdr:row>
-      <xdr:rowOff>67320</xdr:rowOff>
+      <xdr:rowOff>52920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>190080</xdr:colOff>
+      <xdr:colOff>189360</xdr:colOff>
       <xdr:row>76</xdr:row>
-      <xdr:rowOff>114480</xdr:rowOff>
+      <xdr:rowOff>99360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1109,7 +1091,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="12731760"/>
-          <a:ext cx="7543080" cy="2607480"/>
+          <a:ext cx="7527240" cy="2606760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1126,13 +1108,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>22320</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>89640</xdr:rowOff>
+      <xdr:rowOff>75240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>203040</xdr:colOff>
+      <xdr:colOff>202320</xdr:colOff>
       <xdr:row>61</xdr:row>
-      <xdr:rowOff>45000</xdr:rowOff>
+      <xdr:rowOff>29880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1146,7 +1128,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="22320" y="9462240"/>
-          <a:ext cx="7533720" cy="3064320"/>
+          <a:ext cx="7517880" cy="3063600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1163,13 +1145,13 @@
       <xdr:col>12</xdr:col>
       <xdr:colOff>493200</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>56160</xdr:rowOff>
+      <xdr:rowOff>41760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>3240</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>2160</xdr:rowOff>
+      <xdr:colOff>2520</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>169920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1182,8 +1164,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7846200" y="9428760"/>
-          <a:ext cx="7476120" cy="3054960"/>
+          <a:off x="7831080" y="9428760"/>
+          <a:ext cx="7458840" cy="3054240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1200,13 +1182,13 @@
       <xdr:col>25</xdr:col>
       <xdr:colOff>67320</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>123120</xdr:rowOff>
+      <xdr:rowOff>108720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
-      <xdr:colOff>257400</xdr:colOff>
+      <xdr:colOff>256680</xdr:colOff>
       <xdr:row>61</xdr:row>
-      <xdr:rowOff>88200</xdr:rowOff>
+      <xdr:rowOff>73080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1219,8 +1201,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15386400" y="9495720"/>
-          <a:ext cx="7543440" cy="3074040"/>
+          <a:off x="15354720" y="9495720"/>
+          <a:ext cx="7527600" cy="3073320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1237,13 +1219,13 @@
       <xdr:col>37</xdr:col>
       <xdr:colOff>291240</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>134640</xdr:rowOff>
+      <xdr:rowOff>120240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>49</xdr:col>
-      <xdr:colOff>491040</xdr:colOff>
+      <xdr:colOff>490320</xdr:colOff>
       <xdr:row>61</xdr:row>
-      <xdr:rowOff>109080</xdr:rowOff>
+      <xdr:rowOff>93960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1256,8 +1238,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="22963680" y="9507240"/>
-          <a:ext cx="7553160" cy="3083400"/>
+          <a:off x="22916880" y="9507240"/>
+          <a:ext cx="7536960" cy="3082680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1274,13 +1256,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>77</xdr:row>
-      <xdr:rowOff>100800</xdr:rowOff>
+      <xdr:rowOff>86400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>190080</xdr:colOff>
+      <xdr:colOff>189360</xdr:colOff>
       <xdr:row>91</xdr:row>
-      <xdr:rowOff>100440</xdr:rowOff>
+      <xdr:rowOff>85320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1294,7 +1276,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="15508440"/>
-          <a:ext cx="7543080" cy="2559960"/>
+          <a:ext cx="7527240" cy="2559240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1311,13 +1293,13 @@
       <xdr:col>12</xdr:col>
       <xdr:colOff>392040</xdr:colOff>
       <xdr:row>77</xdr:row>
-      <xdr:rowOff>89640</xdr:rowOff>
+      <xdr:rowOff>75240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>601200</xdr:colOff>
+      <xdr:colOff>600480</xdr:colOff>
       <xdr:row>91</xdr:row>
-      <xdr:rowOff>136800</xdr:rowOff>
+      <xdr:rowOff>121680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1330,8 +1312,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7745040" y="15497280"/>
-          <a:ext cx="7562520" cy="2607480"/>
+          <a:off x="7729920" y="15497280"/>
+          <a:ext cx="7546680" cy="2606760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1354,12 +1336,12 @@
   <dimension ref="A4:X44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Z33" activeCellId="0" sqref="Z33"/>
+      <selection pane="topLeft" activeCell="A108" activeCellId="0" sqref="A108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1367,7 +1349,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1384,194 +1366,197 @@
       <c r="I5" s="4" t="n">
         <v>2.4</v>
       </c>
+      <c r="L5" s="5" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="5"/>
-      <c r="C6" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="7" t="n">
+      <c r="B6" s="6"/>
+      <c r="C6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="8" t="n">
         <v>4.41</v>
       </c>
-      <c r="H6" s="8"/>
-      <c r="I6" s="9" t="n">
+      <c r="H6" s="9"/>
+      <c r="I6" s="10" t="n">
         <v>4.4</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
       <c r="G7" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H7" s="3"/>
-      <c r="I7" s="9" t="n">
+      <c r="I7" s="10" t="n">
         <v>1.2</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="11"/>
-      <c r="C8" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="7" t="n">
+      <c r="B8" s="12"/>
+      <c r="C8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="8" t="n">
         <v>4.31</v>
       </c>
-      <c r="H8" s="13"/>
-      <c r="I8" s="9" t="n">
+      <c r="H8" s="14"/>
+      <c r="I8" s="10" t="n">
         <v>4.92</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="14" t="s">
-        <v>5</v>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11" t="s">
+        <v>6</v>
       </c>
       <c r="H9" s="3"/>
-      <c r="I9" s="9" t="n">
+      <c r="I9" s="10" t="n">
         <v>1.2</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="11"/>
-      <c r="C10" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="7" t="n">
+      <c r="B10" s="12"/>
+      <c r="C10" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="8" t="n">
         <v>4.09</v>
       </c>
-      <c r="H10" s="13"/>
-      <c r="I10" s="9" t="n">
+      <c r="H10" s="14"/>
+      <c r="I10" s="10" t="n">
         <v>6.14</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="14" t="s">
-        <v>5</v>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11" t="s">
+        <v>6</v>
       </c>
       <c r="H11" s="3"/>
-      <c r="I11" s="9" t="n">
+      <c r="I11" s="10" t="n">
         <v>1.2</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="11"/>
-      <c r="C12" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="7" t="n">
+      <c r="B12" s="12"/>
+      <c r="C12" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="8" t="n">
         <v>4.31</v>
       </c>
-      <c r="H12" s="13"/>
-      <c r="I12" s="9" t="n">
+      <c r="H12" s="14"/>
+      <c r="I12" s="10" t="n">
         <v>4.92</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="14" t="s">
-        <v>5</v>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11" t="s">
+        <v>6</v>
       </c>
       <c r="H13" s="3"/>
-      <c r="I13" s="9" t="n">
+      <c r="I13" s="10" t="n">
         <v>1.2</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="11"/>
-      <c r="C14" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="7" t="n">
+      <c r="B14" s="12"/>
+      <c r="C14" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="8" t="n">
         <v>4.09</v>
       </c>
-      <c r="H14" s="13"/>
-      <c r="I14" s="9" t="n">
+      <c r="H14" s="14"/>
+      <c r="I14" s="10" t="n">
         <v>6.14</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="14" t="s">
-        <v>5</v>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11" t="s">
+        <v>6</v>
       </c>
       <c r="H15" s="3"/>
-      <c r="I15" s="9" t="n">
+      <c r="I15" s="10" t="n">
         <v>1.2</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="15"/>
-      <c r="C16" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="9" t="n">
+      <c r="C16" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="10" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C17" s="16" t="s">
         <v>1</v>
@@ -1580,32 +1565,32 @@
       <c r="E17" s="16"/>
       <c r="F17" s="16"/>
       <c r="G17" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H17" s="3"/>
-      <c r="I17" s="9" t="n">
+      <c r="I17" s="10" t="n">
         <v>1.2</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="11"/>
-      <c r="C18" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="7" t="n">
+      <c r="B18" s="12"/>
+      <c r="C18" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="8" t="n">
         <v>4.09</v>
       </c>
-      <c r="H18" s="13"/>
-      <c r="I18" s="9" t="n">
+      <c r="H18" s="14"/>
+      <c r="I18" s="10" t="n">
         <v>6.14</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C19" s="16" t="s">
         <v>1</v>
@@ -1614,32 +1599,32 @@
       <c r="E19" s="16"/>
       <c r="F19" s="16"/>
       <c r="G19" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H19" s="3"/>
-      <c r="I19" s="9" t="n">
+      <c r="I19" s="10" t="n">
         <v>1.2</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="11"/>
-      <c r="C20" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="7" t="n">
+      <c r="B20" s="12"/>
+      <c r="C20" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="8" t="n">
         <v>4.31</v>
       </c>
-      <c r="H20" s="13"/>
-      <c r="I20" s="9" t="n">
+      <c r="H20" s="14"/>
+      <c r="I20" s="10" t="n">
         <v>4.92</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C21" s="16" t="s">
         <v>1</v>
@@ -1648,32 +1633,32 @@
       <c r="E21" s="16"/>
       <c r="F21" s="16"/>
       <c r="G21" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H21" s="3"/>
-      <c r="I21" s="9" t="n">
+      <c r="I21" s="10" t="n">
         <v>1.2</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="11"/>
-      <c r="C22" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="7" t="n">
+      <c r="B22" s="12"/>
+      <c r="C22" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="8" t="n">
         <v>4.09</v>
       </c>
-      <c r="H22" s="13"/>
-      <c r="I22" s="9" t="n">
+      <c r="H22" s="14"/>
+      <c r="I22" s="10" t="n">
         <v>6.14</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C23" s="16" t="s">
         <v>1</v>
@@ -1682,32 +1667,32 @@
       <c r="E23" s="16"/>
       <c r="F23" s="16"/>
       <c r="G23" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H23" s="3"/>
-      <c r="I23" s="9" t="n">
+      <c r="I23" s="10" t="n">
         <v>1.2</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="11"/>
-      <c r="C24" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="7" t="n">
+      <c r="B24" s="12"/>
+      <c r="C24" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="8" t="n">
         <v>4.31</v>
       </c>
-      <c r="H24" s="13"/>
-      <c r="I24" s="9" t="n">
+      <c r="H24" s="14"/>
+      <c r="I24" s="10" t="n">
         <v>4.92</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C25" s="16" t="s">
         <v>1</v>
@@ -1716,32 +1701,32 @@
       <c r="E25" s="16"/>
       <c r="F25" s="16"/>
       <c r="G25" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H25" s="3"/>
-      <c r="I25" s="9" t="n">
+      <c r="I25" s="10" t="n">
         <v>1.2</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="11"/>
-      <c r="C26" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="7" t="n">
+      <c r="B26" s="12"/>
+      <c r="C26" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="8" t="n">
         <v>4.49</v>
       </c>
-      <c r="H26" s="13"/>
-      <c r="I26" s="9" t="n">
+      <c r="H26" s="14"/>
+      <c r="I26" s="10" t="n">
         <v>4.4</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C27" s="18" t="s">
         <v>1</v>
@@ -1750,7 +1735,7 @@
       <c r="E27" s="18"/>
       <c r="F27" s="18"/>
       <c r="G27" s="19" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H27" s="19"/>
       <c r="I27" s="20" t="n">
@@ -1758,690 +1743,690 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I28" s="21" t="n">
+      <c r="I28" s="10" t="n">
         <v>0.7</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="30" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="22"/>
-      <c r="B30" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="C30" s="23"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="23" t="s">
+      <c r="A30" s="21"/>
+      <c r="B30" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="H30" s="23"/>
-      <c r="I30" s="24"/>
-      <c r="J30" s="23" t="s">
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="K30" s="23"/>
-      <c r="L30" s="23"/>
-      <c r="M30" s="24"/>
-      <c r="N30" s="23" t="s">
+      <c r="H30" s="22"/>
+      <c r="I30" s="23"/>
+      <c r="J30" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="O30" s="23"/>
-      <c r="P30" s="25"/>
-      <c r="Q30" s="24"/>
-      <c r="R30" s="23" t="s">
+      <c r="K30" s="22"/>
+      <c r="L30" s="22"/>
+      <c r="M30" s="23"/>
+      <c r="N30" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="S30" s="23"/>
-      <c r="T30" s="25"/>
-      <c r="U30" s="24"/>
-      <c r="V30" s="23" t="s">
+      <c r="O30" s="22"/>
+      <c r="P30" s="24"/>
+      <c r="Q30" s="23"/>
+      <c r="R30" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="W30" s="23"/>
-      <c r="X30" s="25"/>
-    </row>
-    <row r="31" s="28" customFormat="true" ht="46.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="26" t="s">
+      <c r="S30" s="22"/>
+      <c r="T30" s="24"/>
+      <c r="U30" s="23"/>
+      <c r="V30" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="26" t="s">
+      <c r="W30" s="22"/>
+      <c r="X30" s="24"/>
+    </row>
+    <row r="31" s="27" customFormat="true" ht="46.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="26" t="s">
+      <c r="B31" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="D31" s="26" t="s">
+      <c r="C31" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="E31" s="26" t="s">
+      <c r="D31" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="F31" s="27"/>
-      <c r="G31" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="H31" s="26" t="s">
+      <c r="E31" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="F31" s="26"/>
+      <c r="G31" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="I31" s="27"/>
-      <c r="J31" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="K31" s="26" t="s">
+      <c r="H31" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="I31" s="26"/>
+      <c r="J31" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="L31" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="M31" s="27"/>
-      <c r="N31" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="O31" s="26" t="s">
+      <c r="K31" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="L31" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="M31" s="26"/>
+      <c r="N31" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="P31" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q31" s="27"/>
-      <c r="R31" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="S31" s="26" t="s">
+      <c r="O31" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="P31" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q31" s="26"/>
+      <c r="R31" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="T31" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="U31" s="27"/>
-      <c r="V31" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="W31" s="26" t="s">
+      <c r="S31" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="T31" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="U31" s="26"/>
+      <c r="V31" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="X31" s="26" t="s">
-        <v>31</v>
+      <c r="W31" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="X31" s="25" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="B32" s="29" t="n">
+      <c r="A32" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" s="28" t="n">
         <v>40</v>
       </c>
-      <c r="C32" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="D32" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="E32" s="29" t="s">
+      <c r="C32" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="F32" s="29"/>
-      <c r="G32" s="29" t="n">
+      <c r="D32" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="F32" s="28"/>
+      <c r="G32" s="28" t="n">
         <v>50</v>
       </c>
-      <c r="H32" s="30" t="s">
+      <c r="H32" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="I32" s="28"/>
+      <c r="J32" s="28" t="n">
+        <v>100</v>
+      </c>
+      <c r="K32" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="L32" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="M32" s="28"/>
+      <c r="N32" s="28" t="n">
+        <v>90</v>
+      </c>
+      <c r="O32" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="P32" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q32" s="28"/>
+      <c r="R32" s="28" t="n">
+        <v>85</v>
+      </c>
+      <c r="S32" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="T32" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="U32" s="28"/>
+      <c r="V32" s="28" t="n">
+        <v>80</v>
+      </c>
+      <c r="W32" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="X32" s="30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="31"/>
+      <c r="B33" s="31"/>
+      <c r="C33" s="31"/>
+      <c r="D33" s="31"/>
+      <c r="E33" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="I32" s="29"/>
-      <c r="J32" s="29" t="n">
+      <c r="F33" s="31"/>
+      <c r="G33" s="31"/>
+      <c r="H33" s="31"/>
+      <c r="I33" s="31"/>
+      <c r="J33" s="31"/>
+      <c r="K33" s="31"/>
+      <c r="L33" s="31"/>
+      <c r="M33" s="31"/>
+      <c r="N33" s="31"/>
+      <c r="O33" s="31"/>
+      <c r="P33" s="32"/>
+      <c r="Q33" s="31"/>
+      <c r="R33" s="31"/>
+      <c r="S33" s="31"/>
+      <c r="T33" s="32"/>
+      <c r="U33" s="31"/>
+      <c r="V33" s="31"/>
+      <c r="W33" s="31"/>
+      <c r="X33" s="32"/>
+    </row>
+    <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" s="33" t="n">
+        <v>40</v>
+      </c>
+      <c r="C34" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="D34" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="E34" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="F34" s="33"/>
+      <c r="G34" s="33" t="n">
+        <v>50</v>
+      </c>
+      <c r="H34" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="I34" s="33"/>
+      <c r="J34" s="33" t="n">
         <v>100</v>
       </c>
-      <c r="K32" s="30" t="s">
+      <c r="K34" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="L34" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="M34" s="33"/>
+      <c r="N34" s="33" t="n">
+        <v>90</v>
+      </c>
+      <c r="O34" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="P34" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q34" s="33"/>
+      <c r="R34" s="33" t="n">
+        <v>85</v>
+      </c>
+      <c r="S34" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="T34" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="U34" s="33"/>
+      <c r="V34" s="33" t="n">
+        <v>80</v>
+      </c>
+      <c r="W34" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="X34" s="34" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="31"/>
+      <c r="B35" s="31"/>
+      <c r="C35" s="31"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="L32" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="M32" s="29"/>
-      <c r="N32" s="29" t="n">
+      <c r="F35" s="31"/>
+      <c r="G35" s="31"/>
+      <c r="H35" s="31"/>
+      <c r="I35" s="31"/>
+      <c r="J35" s="31"/>
+      <c r="K35" s="31"/>
+      <c r="L35" s="31"/>
+      <c r="M35" s="31"/>
+      <c r="N35" s="31"/>
+      <c r="O35" s="31"/>
+      <c r="P35" s="31"/>
+      <c r="Q35" s="31"/>
+      <c r="R35" s="31"/>
+      <c r="S35" s="31"/>
+      <c r="T35" s="31"/>
+      <c r="U35" s="31"/>
+      <c r="V35" s="31"/>
+      <c r="W35" s="31"/>
+      <c r="X35" s="31"/>
+    </row>
+    <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="B36" s="33" t="n">
+        <v>40</v>
+      </c>
+      <c r="C36" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="D36" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="E36" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="F36" s="33"/>
+      <c r="G36" s="33" t="n">
+        <v>50</v>
+      </c>
+      <c r="H36" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="I36" s="33"/>
+      <c r="J36" s="33" t="n">
+        <v>100</v>
+      </c>
+      <c r="K36" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="L36" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="M36" s="33"/>
+      <c r="N36" s="33" t="n">
         <v>90</v>
       </c>
-      <c r="O32" s="30" t="s">
+      <c r="O36" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="P36" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q36" s="33"/>
+      <c r="R36" s="33" t="n">
+        <v>85</v>
+      </c>
+      <c r="S36" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="T36" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="U36" s="33"/>
+      <c r="V36" s="33" t="n">
+        <v>80</v>
+      </c>
+      <c r="W36" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="X36" s="34" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="31"/>
+      <c r="B37" s="31"/>
+      <c r="C37" s="31"/>
+      <c r="D37" s="31"/>
+      <c r="E37" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="F37" s="31"/>
+      <c r="G37" s="31"/>
+      <c r="H37" s="31"/>
+      <c r="I37" s="31"/>
+      <c r="J37" s="31"/>
+      <c r="K37" s="31"/>
+      <c r="L37" s="31"/>
+      <c r="M37" s="31"/>
+      <c r="N37" s="31"/>
+      <c r="O37" s="31"/>
+      <c r="P37" s="31"/>
+      <c r="Q37" s="31"/>
+      <c r="R37" s="31"/>
+      <c r="S37" s="31"/>
+      <c r="T37" s="31"/>
+      <c r="U37" s="31"/>
+      <c r="V37" s="31"/>
+      <c r="W37" s="31"/>
+      <c r="X37" s="31"/>
+    </row>
+    <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="31"/>
+      <c r="B38" s="31"/>
+      <c r="C38" s="31"/>
+      <c r="D38" s="31"/>
+      <c r="E38" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="F38" s="31"/>
+      <c r="G38" s="31"/>
+      <c r="H38" s="31"/>
+      <c r="I38" s="31"/>
+      <c r="J38" s="31"/>
+      <c r="K38" s="31"/>
+      <c r="L38" s="31"/>
+      <c r="M38" s="31"/>
+      <c r="N38" s="31"/>
+      <c r="O38" s="31"/>
+      <c r="P38" s="31"/>
+      <c r="Q38" s="31"/>
+      <c r="R38" s="31"/>
+      <c r="S38" s="31"/>
+      <c r="T38" s="31"/>
+      <c r="U38" s="31"/>
+      <c r="V38" s="31"/>
+      <c r="W38" s="31"/>
+      <c r="X38" s="31"/>
+    </row>
+    <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="B39" s="33" t="n">
+        <v>40</v>
+      </c>
+      <c r="C39" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="D39" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="E39" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="F39" s="33"/>
+      <c r="G39" s="33" t="n">
+        <v>50</v>
+      </c>
+      <c r="H39" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="I39" s="33"/>
+      <c r="J39" s="33" t="n">
+        <v>100</v>
+      </c>
+      <c r="K39" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="L39" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="M39" s="33"/>
+      <c r="N39" s="33" t="n">
+        <v>90</v>
+      </c>
+      <c r="O39" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="P39" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q39" s="33"/>
+      <c r="R39" s="33" t="n">
+        <v>85</v>
+      </c>
+      <c r="S39" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="T39" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="U39" s="33"/>
+      <c r="V39" s="33" t="n">
+        <v>80</v>
+      </c>
+      <c r="W39" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="X39" s="34" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="31"/>
+      <c r="B40" s="31"/>
+      <c r="C40" s="31"/>
+      <c r="D40" s="31"/>
+      <c r="E40" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="F40" s="31"/>
+      <c r="G40" s="31"/>
+      <c r="H40" s="31"/>
+      <c r="I40" s="31"/>
+      <c r="J40" s="31"/>
+      <c r="K40" s="31"/>
+      <c r="L40" s="31"/>
+      <c r="M40" s="31"/>
+      <c r="N40" s="31"/>
+      <c r="O40" s="31"/>
+      <c r="P40" s="31"/>
+      <c r="Q40" s="31"/>
+      <c r="R40" s="31"/>
+      <c r="S40" s="31"/>
+      <c r="T40" s="31"/>
+      <c r="U40" s="31"/>
+      <c r="V40" s="31"/>
+      <c r="W40" s="31"/>
+      <c r="X40" s="31"/>
+    </row>
+    <row r="41" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="B41" s="33" t="n">
+        <v>40</v>
+      </c>
+      <c r="C41" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="D41" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="E41" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="F41" s="33"/>
+      <c r="G41" s="33" t="n">
+        <v>50</v>
+      </c>
+      <c r="H41" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="I41" s="33"/>
+      <c r="J41" s="33" t="n">
+        <v>100</v>
+      </c>
+      <c r="K41" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="L41" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="M41" s="33"/>
+      <c r="N41" s="33" t="n">
+        <v>90</v>
+      </c>
+      <c r="O41" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="P41" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q41" s="33"/>
+      <c r="R41" s="33" t="n">
+        <v>85</v>
+      </c>
+      <c r="S41" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="T41" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="U41" s="33"/>
+      <c r="V41" s="33" t="n">
+        <v>80</v>
+      </c>
+      <c r="W41" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="X41" s="34" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="31"/>
+      <c r="B42" s="31"/>
+      <c r="C42" s="31"/>
+      <c r="D42" s="31"/>
+      <c r="E42" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="F42" s="31"/>
+      <c r="G42" s="31"/>
+      <c r="H42" s="31"/>
+      <c r="I42" s="31"/>
+      <c r="J42" s="31"/>
+      <c r="K42" s="31"/>
+      <c r="L42" s="31"/>
+      <c r="M42" s="31"/>
+      <c r="N42" s="31"/>
+      <c r="O42" s="31"/>
+      <c r="P42" s="32"/>
+      <c r="Q42" s="31"/>
+      <c r="R42" s="31"/>
+      <c r="S42" s="31"/>
+      <c r="T42" s="32"/>
+      <c r="U42" s="31"/>
+      <c r="V42" s="31"/>
+      <c r="W42" s="31"/>
+      <c r="X42" s="32"/>
+    </row>
+    <row r="43" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B43" s="28" t="n">
+        <v>40</v>
+      </c>
+      <c r="C43" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="D43" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E43" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="F43" s="28"/>
+      <c r="G43" s="28" t="n">
+        <v>50</v>
+      </c>
+      <c r="H43" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="P32" s="29" t="s">
+      <c r="I43" s="28"/>
+      <c r="J43" s="28" t="n">
+        <v>100</v>
+      </c>
+      <c r="K43" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="L43" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="M43" s="28"/>
+      <c r="N43" s="28" t="n">
+        <v>90</v>
+      </c>
+      <c r="O43" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="Q32" s="29"/>
-      <c r="R32" s="29" t="n">
+      <c r="P43" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q43" s="28"/>
+      <c r="R43" s="28" t="n">
         <v>85</v>
       </c>
-      <c r="S32" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="T32" s="31" t="s">
+      <c r="S43" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="U32" s="29"/>
-      <c r="V32" s="29" t="n">
+      <c r="T43" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="U43" s="28"/>
+      <c r="V43" s="28" t="n">
         <v>80</v>
       </c>
-      <c r="W32" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="X32" s="31" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="32"/>
-      <c r="B33" s="32"/>
-      <c r="C33" s="32"/>
-      <c r="D33" s="32"/>
-      <c r="E33" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="F33" s="32"/>
-      <c r="G33" s="32"/>
-      <c r="H33" s="32"/>
-      <c r="I33" s="32"/>
-      <c r="J33" s="32"/>
-      <c r="K33" s="32"/>
-      <c r="L33" s="32"/>
-      <c r="M33" s="32"/>
-      <c r="N33" s="32"/>
-      <c r="O33" s="32"/>
-      <c r="P33" s="33"/>
-      <c r="Q33" s="32"/>
-      <c r="R33" s="32"/>
-      <c r="S33" s="32"/>
-      <c r="T33" s="33"/>
-      <c r="U33" s="32"/>
-      <c r="V33" s="32"/>
-      <c r="W33" s="32"/>
-      <c r="X33" s="33"/>
-    </row>
-    <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="B34" s="34" t="n">
-        <v>40</v>
-      </c>
-      <c r="C34" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="D34" s="34" t="s">
-        <v>40</v>
-      </c>
-      <c r="E34" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="F34" s="34"/>
-      <c r="G34" s="34" t="n">
-        <v>50</v>
-      </c>
-      <c r="H34" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="I34" s="34"/>
-      <c r="J34" s="34" t="n">
-        <v>100</v>
-      </c>
-      <c r="K34" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="L34" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="M34" s="34"/>
-      <c r="N34" s="34" t="n">
-        <v>90</v>
-      </c>
-      <c r="O34" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="P34" s="35" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q34" s="34"/>
-      <c r="R34" s="34" t="n">
-        <v>85</v>
-      </c>
-      <c r="S34" s="34" t="s">
-        <v>45</v>
-      </c>
-      <c r="T34" s="35" t="s">
-        <v>44</v>
-      </c>
-      <c r="U34" s="34"/>
-      <c r="V34" s="34" t="n">
-        <v>80</v>
-      </c>
-      <c r="W34" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="X34" s="35" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="32"/>
-      <c r="B35" s="32"/>
-      <c r="C35" s="32"/>
-      <c r="D35" s="32"/>
-      <c r="E35" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="F35" s="32"/>
-      <c r="G35" s="32"/>
-      <c r="H35" s="32"/>
-      <c r="I35" s="32"/>
-      <c r="J35" s="32"/>
-      <c r="K35" s="32"/>
-      <c r="L35" s="32"/>
-      <c r="M35" s="32"/>
-      <c r="N35" s="32"/>
-      <c r="O35" s="32"/>
-      <c r="P35" s="32"/>
-      <c r="Q35" s="32"/>
-      <c r="R35" s="32"/>
-      <c r="S35" s="32"/>
-      <c r="T35" s="32"/>
-      <c r="U35" s="32"/>
-      <c r="V35" s="32"/>
-      <c r="W35" s="32"/>
-      <c r="X35" s="32"/>
-    </row>
-    <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="B36" s="34" t="n">
-        <v>40</v>
-      </c>
-      <c r="C36" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="D36" s="34" t="s">
-        <v>48</v>
-      </c>
-      <c r="E36" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="F36" s="34"/>
-      <c r="G36" s="34" t="n">
-        <v>50</v>
-      </c>
-      <c r="H36" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="I36" s="34"/>
-      <c r="J36" s="34" t="n">
-        <v>100</v>
-      </c>
-      <c r="K36" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="L36" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="M36" s="34"/>
-      <c r="N36" s="34" t="n">
-        <v>90</v>
-      </c>
-      <c r="O36" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="P36" s="35" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q36" s="34"/>
-      <c r="R36" s="34" t="n">
-        <v>85</v>
-      </c>
-      <c r="S36" s="34" t="s">
-        <v>45</v>
-      </c>
-      <c r="T36" s="35" t="s">
-        <v>44</v>
-      </c>
-      <c r="U36" s="34"/>
-      <c r="V36" s="34" t="n">
-        <v>80</v>
-      </c>
-      <c r="W36" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="X36" s="35" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="32"/>
-      <c r="B37" s="32"/>
-      <c r="C37" s="32"/>
-      <c r="D37" s="32"/>
-      <c r="E37" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="F37" s="32"/>
-      <c r="G37" s="32"/>
-      <c r="H37" s="32"/>
-      <c r="I37" s="32"/>
-      <c r="J37" s="32"/>
-      <c r="K37" s="32"/>
-      <c r="L37" s="32"/>
-      <c r="M37" s="32"/>
-      <c r="N37" s="32"/>
-      <c r="O37" s="32"/>
-      <c r="P37" s="32"/>
-      <c r="Q37" s="32"/>
-      <c r="R37" s="32"/>
-      <c r="S37" s="32"/>
-      <c r="T37" s="32"/>
-      <c r="U37" s="32"/>
-      <c r="V37" s="32"/>
-      <c r="W37" s="32"/>
-      <c r="X37" s="32"/>
-    </row>
-    <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="32"/>
-      <c r="B38" s="32"/>
-      <c r="C38" s="32"/>
-      <c r="D38" s="32"/>
-      <c r="E38" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="F38" s="32"/>
-      <c r="G38" s="32"/>
-      <c r="H38" s="32"/>
-      <c r="I38" s="32"/>
-      <c r="J38" s="32"/>
-      <c r="K38" s="32"/>
-      <c r="L38" s="32"/>
-      <c r="M38" s="32"/>
-      <c r="N38" s="32"/>
-      <c r="O38" s="32"/>
-      <c r="P38" s="32"/>
-      <c r="Q38" s="32"/>
-      <c r="R38" s="32"/>
-      <c r="S38" s="32"/>
-      <c r="T38" s="32"/>
-      <c r="U38" s="32"/>
-      <c r="V38" s="32"/>
-      <c r="W38" s="32"/>
-      <c r="X38" s="32"/>
-    </row>
-    <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="B39" s="34" t="n">
-        <v>40</v>
-      </c>
-      <c r="C39" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="D39" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="E39" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="F39" s="34"/>
-      <c r="G39" s="34" t="n">
-        <v>50</v>
-      </c>
-      <c r="H39" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="I39" s="34"/>
-      <c r="J39" s="34" t="n">
-        <v>100</v>
-      </c>
-      <c r="K39" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="L39" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="M39" s="34"/>
-      <c r="N39" s="34" t="n">
-        <v>90</v>
-      </c>
-      <c r="O39" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="P39" s="35" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q39" s="34"/>
-      <c r="R39" s="34" t="n">
-        <v>85</v>
-      </c>
-      <c r="S39" s="34" t="s">
-        <v>45</v>
-      </c>
-      <c r="T39" s="35" t="s">
-        <v>44</v>
-      </c>
-      <c r="U39" s="34"/>
-      <c r="V39" s="34" t="n">
-        <v>80</v>
-      </c>
-      <c r="W39" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="X39" s="35" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="32"/>
-      <c r="B40" s="32"/>
-      <c r="C40" s="32"/>
-      <c r="D40" s="32"/>
-      <c r="E40" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="F40" s="32"/>
-      <c r="G40" s="32"/>
-      <c r="H40" s="32"/>
-      <c r="I40" s="32"/>
-      <c r="J40" s="32"/>
-      <c r="K40" s="32"/>
-      <c r="L40" s="32"/>
-      <c r="M40" s="32"/>
-      <c r="N40" s="32"/>
-      <c r="O40" s="32"/>
-      <c r="P40" s="32"/>
-      <c r="Q40" s="32"/>
-      <c r="R40" s="32"/>
-      <c r="S40" s="32"/>
-      <c r="T40" s="32"/>
-      <c r="U40" s="32"/>
-      <c r="V40" s="32"/>
-      <c r="W40" s="32"/>
-      <c r="X40" s="32"/>
-    </row>
-    <row r="41" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="B41" s="34" t="n">
-        <v>40</v>
-      </c>
-      <c r="C41" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="D41" s="34" t="s">
-        <v>50</v>
-      </c>
-      <c r="E41" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="F41" s="34"/>
-      <c r="G41" s="34" t="n">
-        <v>50</v>
-      </c>
-      <c r="H41" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="I41" s="34"/>
-      <c r="J41" s="34" t="n">
-        <v>100</v>
-      </c>
-      <c r="K41" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="L41" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="M41" s="34"/>
-      <c r="N41" s="34" t="n">
-        <v>90</v>
-      </c>
-      <c r="O41" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="P41" s="35" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q41" s="34"/>
-      <c r="R41" s="34" t="n">
-        <v>85</v>
-      </c>
-      <c r="S41" s="34" t="s">
-        <v>45</v>
-      </c>
-      <c r="T41" s="35" t="s">
-        <v>44</v>
-      </c>
-      <c r="U41" s="34"/>
-      <c r="V41" s="34" t="n">
-        <v>80</v>
-      </c>
-      <c r="W41" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="X41" s="35" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="32"/>
-      <c r="B42" s="32"/>
-      <c r="C42" s="32"/>
-      <c r="D42" s="32"/>
-      <c r="E42" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="F42" s="32"/>
-      <c r="G42" s="32"/>
-      <c r="H42" s="32"/>
-      <c r="I42" s="32"/>
-      <c r="J42" s="32"/>
-      <c r="K42" s="32"/>
-      <c r="L42" s="32"/>
-      <c r="M42" s="32"/>
-      <c r="N42" s="32"/>
-      <c r="O42" s="32"/>
-      <c r="P42" s="33"/>
-      <c r="Q42" s="32"/>
-      <c r="R42" s="32"/>
-      <c r="S42" s="32"/>
-      <c r="T42" s="33"/>
-      <c r="U42" s="32"/>
-      <c r="V42" s="32"/>
-      <c r="W42" s="32"/>
-      <c r="X42" s="33"/>
-    </row>
-    <row r="43" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="29" t="s">
-        <v>51</v>
-      </c>
-      <c r="B43" s="29" t="n">
-        <v>40</v>
-      </c>
-      <c r="C43" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="D43" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="E43" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="F43" s="29"/>
-      <c r="G43" s="29" t="n">
-        <v>50</v>
-      </c>
-      <c r="H43" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="I43" s="29"/>
-      <c r="J43" s="29" t="n">
-        <v>100</v>
-      </c>
-      <c r="K43" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="L43" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="M43" s="29"/>
-      <c r="N43" s="29" t="n">
-        <v>90</v>
-      </c>
-      <c r="O43" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="P43" s="29" t="s">
+      <c r="W43" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="X43" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="Q43" s="29"/>
-      <c r="R43" s="29" t="n">
-        <v>85</v>
-      </c>
-      <c r="S43" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="T43" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="U43" s="29"/>
-      <c r="V43" s="29" t="n">
-        <v>80</v>
-      </c>
-      <c r="W43" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="X43" s="31" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
-      <c r="C44" s="36"/>
-      <c r="D44" s="36"/>
-      <c r="E44" s="36"/>
-      <c r="F44" s="37"/>
-      <c r="G44" s="36"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="37"/>
-      <c r="J44" s="36"/>
-      <c r="K44" s="36"/>
-      <c r="L44" s="36"/>
-      <c r="M44" s="37"/>
-      <c r="N44" s="36"/>
-      <c r="O44" s="36"/>
-      <c r="P44" s="38"/>
-      <c r="Q44" s="37"/>
-      <c r="R44" s="36"/>
-      <c r="S44" s="36"/>
-      <c r="T44" s="38"/>
-      <c r="U44" s="37"/>
-      <c r="V44" s="36"/>
-      <c r="W44" s="36"/>
-      <c r="X44" s="38"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
+      <c r="C44" s="35"/>
+      <c r="D44" s="35"/>
+      <c r="E44" s="35"/>
+      <c r="F44" s="36"/>
+      <c r="G44" s="35"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="35"/>
+      <c r="K44" s="35"/>
+      <c r="L44" s="35"/>
+      <c r="M44" s="36"/>
+      <c r="N44" s="35"/>
+      <c r="O44" s="35"/>
+      <c r="P44" s="37"/>
+      <c r="Q44" s="36"/>
+      <c r="R44" s="35"/>
+      <c r="S44" s="35"/>
+      <c r="T44" s="37"/>
+      <c r="U44" s="36"/>
+      <c r="V44" s="35"/>
+      <c r="W44" s="35"/>
+      <c r="X44" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="31">
@@ -2501,7 +2486,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2527,7 +2512,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>